<commit_message>
Change scraping from Directorate of Health (Eventually move to API which is now available)
</commit_message>
<xml_diff>
--- a/data/01_infected/msis/municipality_wide.xlsx
+++ b/data/01_infected/msis/municipality_wide.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AN359"/>
+  <dimension ref="A1:AO359"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -558,6 +558,11 @@
           <t>2020-04-28</t>
         </is>
       </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>2020-04-29</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -690,6 +695,9 @@
       <c r="AN2">
         <v>2338</v>
       </c>
+      <c r="AO2">
+        <v>2353</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -822,6 +830,9 @@
       <c r="AN3">
         <v>14</v>
       </c>
+      <c r="AO3">
+        <v>14</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -954,6 +965,9 @@
       <c r="AN4">
         <v>132</v>
       </c>
+      <c r="AO4">
+        <v>133</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1086,6 +1100,9 @@
       <c r="AN5">
         <v>51</v>
       </c>
+      <c r="AO5">
+        <v>51</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1218,6 +1235,9 @@
       <c r="AN6">
         <v>47</v>
       </c>
+      <c r="AO6">
+        <v>47</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1350,6 +1370,9 @@
       <c r="AN7">
         <v>5</v>
       </c>
+      <c r="AO7">
+        <v>5</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1482,6 +1505,9 @@
       <c r="AN8">
         <v>1</v>
       </c>
+      <c r="AO8">
+        <v>1</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1614,6 +1640,9 @@
       <c r="AN9">
         <v>0</v>
       </c>
+      <c r="AO9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1746,6 +1775,9 @@
       <c r="AN10">
         <v>7</v>
       </c>
+      <c r="AO10">
+        <v>7</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1878,6 +1910,9 @@
       <c r="AN11">
         <v>6</v>
       </c>
+      <c r="AO11">
+        <v>6</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -2010,6 +2045,9 @@
       <c r="AN12">
         <v>12</v>
       </c>
+      <c r="AO12">
+        <v>12</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -2142,6 +2180,9 @@
       <c r="AN13">
         <v>13</v>
       </c>
+      <c r="AO13">
+        <v>13</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -2274,6 +2315,9 @@
       <c r="AN14">
         <v>16</v>
       </c>
+      <c r="AO14">
+        <v>16</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2406,6 +2450,9 @@
       <c r="AN15">
         <v>11</v>
       </c>
+      <c r="AO15">
+        <v>11</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2538,6 +2585,9 @@
       <c r="AN16">
         <v>13</v>
       </c>
+      <c r="AO16">
+        <v>13</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2670,6 +2720,9 @@
       <c r="AN17">
         <v>0</v>
       </c>
+      <c r="AO17">
+        <v>0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2802,6 +2855,9 @@
       <c r="AN18">
         <v>0</v>
       </c>
+      <c r="AO18">
+        <v>0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2934,6 +2990,9 @@
       <c r="AN19">
         <v>3</v>
       </c>
+      <c r="AO19">
+        <v>3</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -3066,6 +3125,9 @@
       <c r="AN20">
         <v>0</v>
       </c>
+      <c r="AO20">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -3198,6 +3260,9 @@
       <c r="AN21">
         <v>1</v>
       </c>
+      <c r="AO21">
+        <v>1</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -3330,6 +3395,9 @@
       <c r="AN22">
         <v>20</v>
       </c>
+      <c r="AO22">
+        <v>20</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -3462,6 +3530,9 @@
       <c r="AN23">
         <v>59</v>
       </c>
+      <c r="AO23">
+        <v>59</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -3594,6 +3665,9 @@
       <c r="AN24">
         <v>0</v>
       </c>
+      <c r="AO24">
+        <v>0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -3726,6 +3800,9 @@
       <c r="AN25">
         <v>11</v>
       </c>
+      <c r="AO25">
+        <v>11</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -3858,6 +3935,9 @@
       <c r="AN26">
         <v>18</v>
       </c>
+      <c r="AO26">
+        <v>18</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -3990,6 +4070,9 @@
       <c r="AN27">
         <v>13</v>
       </c>
+      <c r="AO27">
+        <v>13</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -4122,6 +4205,9 @@
       <c r="AN28">
         <v>27</v>
       </c>
+      <c r="AO28">
+        <v>27</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -4254,6 +4340,9 @@
       <c r="AN29">
         <v>1</v>
       </c>
+      <c r="AO29">
+        <v>1</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -4386,6 +4475,9 @@
       <c r="AN30">
         <v>5</v>
       </c>
+      <c r="AO30">
+        <v>5</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -4518,6 +4610,9 @@
       <c r="AN31">
         <v>3</v>
       </c>
+      <c r="AO31">
+        <v>3</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -4650,6 +4745,9 @@
       <c r="AN32">
         <v>8</v>
       </c>
+      <c r="AO32">
+        <v>8</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -4782,6 +4880,9 @@
       <c r="AN33">
         <v>2</v>
       </c>
+      <c r="AO33">
+        <v>2</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -4914,6 +5015,9 @@
       <c r="AN34">
         <v>6</v>
       </c>
+      <c r="AO34">
+        <v>6</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -5046,6 +5150,9 @@
       <c r="AN35">
         <v>0</v>
       </c>
+      <c r="AO35">
+        <v>0</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -5178,6 +5285,9 @@
       <c r="AN36">
         <v>1</v>
       </c>
+      <c r="AO36">
+        <v>1</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -5310,6 +5420,9 @@
       <c r="AN37">
         <v>6</v>
       </c>
+      <c r="AO37">
+        <v>6</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -5442,6 +5555,9 @@
       <c r="AN38">
         <v>5</v>
       </c>
+      <c r="AO38">
+        <v>5</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -5574,6 +5690,9 @@
       <c r="AN39">
         <v>1</v>
       </c>
+      <c r="AO39">
+        <v>1</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -5706,6 +5825,9 @@
       <c r="AN40">
         <v>10</v>
       </c>
+      <c r="AO40">
+        <v>10</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -5838,6 +5960,9 @@
       <c r="AN41">
         <v>0</v>
       </c>
+      <c r="AO41">
+        <v>0</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -5970,6 +6095,9 @@
       <c r="AN42">
         <v>0</v>
       </c>
+      <c r="AO42">
+        <v>0</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -6102,6 +6230,9 @@
       <c r="AN43">
         <v>0</v>
       </c>
+      <c r="AO43">
+        <v>1</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -6234,6 +6365,9 @@
       <c r="AN44">
         <v>1</v>
       </c>
+      <c r="AO44">
+        <v>1</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -6366,6 +6500,9 @@
       <c r="AN45">
         <v>2</v>
       </c>
+      <c r="AO45">
+        <v>2</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -6498,6 +6635,9 @@
       <c r="AN46">
         <v>2</v>
       </c>
+      <c r="AO46">
+        <v>2</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -6630,6 +6770,9 @@
       <c r="AN47">
         <v>0</v>
       </c>
+      <c r="AO47">
+        <v>0</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -6762,6 +6905,9 @@
       <c r="AN48">
         <v>3</v>
       </c>
+      <c r="AO48">
+        <v>3</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -6894,6 +7040,9 @@
       <c r="AN49">
         <v>4</v>
       </c>
+      <c r="AO49">
+        <v>4</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -7026,6 +7175,9 @@
       <c r="AN50">
         <v>1</v>
       </c>
+      <c r="AO50">
+        <v>1</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -7158,6 +7310,9 @@
       <c r="AN51">
         <v>3</v>
       </c>
+      <c r="AO51">
+        <v>3</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -7290,6 +7445,9 @@
       <c r="AN52">
         <v>39</v>
       </c>
+      <c r="AO52">
+        <v>39</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -7422,6 +7580,9 @@
       <c r="AN53">
         <v>6</v>
       </c>
+      <c r="AO53">
+        <v>6</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -7554,6 +7715,9 @@
       <c r="AN54">
         <v>0</v>
       </c>
+      <c r="AO54">
+        <v>0</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -7686,6 +7850,9 @@
       <c r="AN55">
         <v>2</v>
       </c>
+      <c r="AO55">
+        <v>2</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -7818,6 +7985,9 @@
       <c r="AN56">
         <v>5</v>
       </c>
+      <c r="AO56">
+        <v>5</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -7950,6 +8120,9 @@
       <c r="AN57">
         <v>3</v>
       </c>
+      <c r="AO57">
+        <v>3</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -8082,6 +8255,9 @@
       <c r="AN58">
         <v>0</v>
       </c>
+      <c r="AO58">
+        <v>0</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -8214,6 +8390,9 @@
       <c r="AN59">
         <v>0</v>
       </c>
+      <c r="AO59">
+        <v>0</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -8346,6 +8525,9 @@
       <c r="AN60">
         <v>2</v>
       </c>
+      <c r="AO60">
+        <v>2</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -8478,6 +8660,9 @@
       <c r="AN61">
         <v>4</v>
       </c>
+      <c r="AO61">
+        <v>4</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -8610,6 +8795,9 @@
       <c r="AN62">
         <v>1</v>
       </c>
+      <c r="AO62">
+        <v>1</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -8742,6 +8930,9 @@
       <c r="AN63">
         <v>1</v>
       </c>
+      <c r="AO63">
+        <v>1</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -8874,6 +9065,9 @@
       <c r="AN64">
         <v>0</v>
       </c>
+      <c r="AO64">
+        <v>0</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -9006,6 +9200,9 @@
       <c r="AN65">
         <v>5</v>
       </c>
+      <c r="AO65">
+        <v>5</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -9138,6 +9335,9 @@
       <c r="AN66">
         <v>0</v>
       </c>
+      <c r="AO66">
+        <v>0</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -9270,6 +9470,9 @@
       <c r="AN67">
         <v>0</v>
       </c>
+      <c r="AO67">
+        <v>0</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -9402,6 +9605,9 @@
       <c r="AN68">
         <v>4</v>
       </c>
+      <c r="AO68">
+        <v>4</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -9534,6 +9740,9 @@
       <c r="AN69">
         <v>0</v>
       </c>
+      <c r="AO69">
+        <v>0</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -9666,6 +9875,9 @@
       <c r="AN70">
         <v>0</v>
       </c>
+      <c r="AO70">
+        <v>0</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -9798,6 +10010,9 @@
       <c r="AN71">
         <v>0</v>
       </c>
+      <c r="AO71">
+        <v>0</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -9930,6 +10145,9 @@
       <c r="AN72">
         <v>5</v>
       </c>
+      <c r="AO72">
+        <v>5</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -10062,6 +10280,9 @@
       <c r="AN73">
         <v>0</v>
       </c>
+      <c r="AO73">
+        <v>0</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -10194,6 +10415,9 @@
       <c r="AN74">
         <v>0</v>
       </c>
+      <c r="AO74">
+        <v>0</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -10326,6 +10550,9 @@
       <c r="AN75">
         <v>0</v>
       </c>
+      <c r="AO75">
+        <v>0</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -10458,6 +10685,9 @@
       <c r="AN76">
         <v>2</v>
       </c>
+      <c r="AO76">
+        <v>2</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -10590,6 +10820,9 @@
       <c r="AN77">
         <v>0</v>
       </c>
+      <c r="AO77">
+        <v>0</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -10722,6 +10955,9 @@
       <c r="AN78">
         <v>1</v>
       </c>
+      <c r="AO78">
+        <v>1</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -10854,6 +11090,9 @@
       <c r="AN79">
         <v>0</v>
       </c>
+      <c r="AO79">
+        <v>0</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -10986,6 +11225,9 @@
       <c r="AN80">
         <v>0</v>
       </c>
+      <c r="AO80">
+        <v>0</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -11118,6 +11360,9 @@
       <c r="AN81">
         <v>0</v>
       </c>
+      <c r="AO81">
+        <v>0</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -11250,6 +11495,9 @@
       <c r="AN82">
         <v>0</v>
       </c>
+      <c r="AO82">
+        <v>0</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -11382,6 +11630,9 @@
       <c r="AN83">
         <v>6</v>
       </c>
+      <c r="AO83">
+        <v>6</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -11514,6 +11765,9 @@
       <c r="AN84">
         <v>13</v>
       </c>
+      <c r="AO84">
+        <v>13</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -11646,6 +11900,9 @@
       <c r="AN85">
         <v>3</v>
       </c>
+      <c r="AO85">
+        <v>3</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -11778,6 +12035,9 @@
       <c r="AN86">
         <v>5</v>
       </c>
+      <c r="AO86">
+        <v>5</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -11910,6 +12170,9 @@
       <c r="AN87">
         <v>0</v>
       </c>
+      <c r="AO87">
+        <v>0</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -12042,6 +12305,9 @@
       <c r="AN88">
         <v>0</v>
       </c>
+      <c r="AO88">
+        <v>0</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -12174,6 +12440,9 @@
       <c r="AN89">
         <v>6</v>
       </c>
+      <c r="AO89">
+        <v>6</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -12306,6 +12575,9 @@
       <c r="AN90">
         <v>0</v>
       </c>
+      <c r="AO90">
+        <v>0</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -12438,6 +12710,9 @@
       <c r="AN91">
         <v>1</v>
       </c>
+      <c r="AO91">
+        <v>1</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -12570,6 +12845,9 @@
       <c r="AN92">
         <v>0</v>
       </c>
+      <c r="AO92">
+        <v>0</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -12702,6 +12980,9 @@
       <c r="AN93">
         <v>35</v>
       </c>
+      <c r="AO93">
+        <v>36</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -12834,6 +13115,9 @@
       <c r="AN94">
         <v>95</v>
       </c>
+      <c r="AO94">
+        <v>97</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -12966,6 +13250,9 @@
       <c r="AN95">
         <v>64</v>
       </c>
+      <c r="AO95">
+        <v>64</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -13098,6 +13385,9 @@
       <c r="AN96">
         <v>87</v>
       </c>
+      <c r="AO96">
+        <v>90</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -13230,6 +13520,9 @@
       <c r="AN97">
         <v>172</v>
       </c>
+      <c r="AO97">
+        <v>172</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -13362,6 +13655,9 @@
       <c r="AN98">
         <v>21</v>
       </c>
+      <c r="AO98">
+        <v>21</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -13494,6 +13790,9 @@
       <c r="AN99">
         <v>10</v>
       </c>
+      <c r="AO99">
+        <v>10</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -13626,6 +13925,9 @@
       <c r="AN100">
         <v>2</v>
       </c>
+      <c r="AO100">
+        <v>2</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -13758,6 +14060,9 @@
       <c r="AN101">
         <v>2</v>
       </c>
+      <c r="AO101">
+        <v>2</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -13890,6 +14195,9 @@
       <c r="AN102">
         <v>3</v>
       </c>
+      <c r="AO102">
+        <v>3</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -14022,6 +14330,9 @@
       <c r="AN103">
         <v>48</v>
       </c>
+      <c r="AO103">
+        <v>48</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -14154,6 +14465,9 @@
       <c r="AN104">
         <v>2</v>
       </c>
+      <c r="AO104">
+        <v>2</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -14286,6 +14600,9 @@
       <c r="AN105">
         <v>1</v>
       </c>
+      <c r="AO105">
+        <v>1</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -14418,6 +14735,9 @@
       <c r="AN106">
         <v>2</v>
       </c>
+      <c r="AO106">
+        <v>2</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -14550,6 +14870,9 @@
       <c r="AN107">
         <v>6</v>
       </c>
+      <c r="AO107">
+        <v>6</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -14682,6 +15005,9 @@
       <c r="AN108">
         <v>23</v>
       </c>
+      <c r="AO108">
+        <v>23</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -14814,6 +15140,9 @@
       <c r="AN109">
         <v>98</v>
       </c>
+      <c r="AO109">
+        <v>100</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -14946,6 +15275,9 @@
       <c r="AN110">
         <v>18</v>
       </c>
+      <c r="AO110">
+        <v>19</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -15078,6 +15410,9 @@
       <c r="AN111">
         <v>22</v>
       </c>
+      <c r="AO111">
+        <v>26</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -15210,6 +15545,9 @@
       <c r="AN112">
         <v>47</v>
       </c>
+      <c r="AO112">
+        <v>47</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -15342,6 +15680,9 @@
       <c r="AN113">
         <v>407</v>
       </c>
+      <c r="AO113">
+        <v>409</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -15474,6 +15815,9 @@
       <c r="AN114">
         <v>176</v>
       </c>
+      <c r="AO114">
+        <v>177</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -15606,6 +15950,9 @@
       <c r="AN115">
         <v>10</v>
       </c>
+      <c r="AO115">
+        <v>10</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -15738,6 +16085,9 @@
       <c r="AN116">
         <v>25</v>
       </c>
+      <c r="AO116">
+        <v>26</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -15870,6 +16220,9 @@
       <c r="AN117">
         <v>49</v>
       </c>
+      <c r="AO117">
+        <v>49</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -16002,6 +16355,9 @@
       <c r="AN118">
         <v>92</v>
       </c>
+      <c r="AO118">
+        <v>92</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -16134,6 +16490,9 @@
       <c r="AN119">
         <v>156</v>
       </c>
+      <c r="AO119">
+        <v>156</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -16266,6 +16625,9 @@
       <c r="AN120">
         <v>45</v>
       </c>
+      <c r="AO120">
+        <v>45</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -16398,6 +16760,9 @@
       <c r="AN121">
         <v>8</v>
       </c>
+      <c r="AO121">
+        <v>8</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -16530,6 +16895,9 @@
       <c r="AN122">
         <v>58</v>
       </c>
+      <c r="AO122">
+        <v>58</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -16662,6 +17030,9 @@
       <c r="AN123">
         <v>14</v>
       </c>
+      <c r="AO123">
+        <v>14</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -16794,6 +17165,9 @@
       <c r="AN124">
         <v>39</v>
       </c>
+      <c r="AO124">
+        <v>39</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -16926,6 +17300,9 @@
       <c r="AN125">
         <v>17</v>
       </c>
+      <c r="AO125">
+        <v>17</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -17058,6 +17435,9 @@
       <c r="AN126">
         <v>2</v>
       </c>
+      <c r="AO126">
+        <v>2</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -17190,6 +17570,9 @@
       <c r="AN127">
         <v>10</v>
       </c>
+      <c r="AO127">
+        <v>10</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -17322,6 +17705,9 @@
       <c r="AN128">
         <v>1</v>
       </c>
+      <c r="AO128">
+        <v>1</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -17454,6 +17840,9 @@
       <c r="AN129">
         <v>7</v>
       </c>
+      <c r="AO129">
+        <v>7</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -17586,6 +17975,9 @@
       <c r="AN130">
         <v>10</v>
       </c>
+      <c r="AO130">
+        <v>11</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -17718,6 +18110,9 @@
       <c r="AN131">
         <v>8</v>
       </c>
+      <c r="AO131">
+        <v>8</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -17850,6 +18245,9 @@
       <c r="AN132">
         <v>13</v>
       </c>
+      <c r="AO132">
+        <v>13</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -17982,6 +18380,9 @@
       <c r="AN133">
         <v>44</v>
       </c>
+      <c r="AO133">
+        <v>44</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -18114,6 +18515,9 @@
       <c r="AN134">
         <v>0</v>
       </c>
+      <c r="AO134">
+        <v>0</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -18246,6 +18650,9 @@
       <c r="AN135">
         <v>0</v>
       </c>
+      <c r="AO135">
+        <v>0</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -18378,6 +18785,9 @@
       <c r="AN136">
         <v>10</v>
       </c>
+      <c r="AO136">
+        <v>10</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -18510,6 +18920,9 @@
       <c r="AN137">
         <v>5</v>
       </c>
+      <c r="AO137">
+        <v>9</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -18642,6 +19055,9 @@
       <c r="AN138">
         <v>42</v>
       </c>
+      <c r="AO138">
+        <v>42</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -18774,6 +19190,9 @@
       <c r="AN139">
         <v>4</v>
       </c>
+      <c r="AO139">
+        <v>4</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -18906,6 +19325,9 @@
       <c r="AN140">
         <v>1</v>
       </c>
+      <c r="AO140">
+        <v>1</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -19038,6 +19460,9 @@
       <c r="AN141">
         <v>3</v>
       </c>
+      <c r="AO141">
+        <v>3</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -19170,6 +19595,9 @@
       <c r="AN142">
         <v>6</v>
       </c>
+      <c r="AO142">
+        <v>6</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -19302,6 +19730,9 @@
       <c r="AN143">
         <v>11</v>
       </c>
+      <c r="AO143">
+        <v>11</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -19434,6 +19865,9 @@
       <c r="AN144">
         <v>2</v>
       </c>
+      <c r="AO144">
+        <v>2</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -19566,6 +20000,9 @@
       <c r="AN145">
         <v>82</v>
       </c>
+      <c r="AO145">
+        <v>82</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -19698,6 +20135,9 @@
       <c r="AN146">
         <v>38</v>
       </c>
+      <c r="AO146">
+        <v>38</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -19830,6 +20270,9 @@
       <c r="AN147">
         <v>22</v>
       </c>
+      <c r="AO147">
+        <v>23</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -19962,6 +20405,9 @@
       <c r="AN148">
         <v>62</v>
       </c>
+      <c r="AO148">
+        <v>62</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -20094,6 +20540,9 @@
       <c r="AN149">
         <v>11</v>
       </c>
+      <c r="AO149">
+        <v>12</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -20226,6 +20675,9 @@
       <c r="AN150">
         <v>35</v>
       </c>
+      <c r="AO150">
+        <v>36</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -20358,6 +20810,9 @@
       <c r="AN151">
         <v>0</v>
       </c>
+      <c r="AO151">
+        <v>0</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -20490,6 +20945,9 @@
       <c r="AN152">
         <v>20</v>
       </c>
+      <c r="AO152">
+        <v>21</v>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -20622,6 +21080,9 @@
       <c r="AN153">
         <v>4</v>
       </c>
+      <c r="AO153">
+        <v>4</v>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -20754,6 +21215,9 @@
       <c r="AN154">
         <v>5</v>
       </c>
+      <c r="AO154">
+        <v>5</v>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -20886,6 +21350,9 @@
       <c r="AN155">
         <v>3</v>
       </c>
+      <c r="AO155">
+        <v>3</v>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -21018,6 +21485,9 @@
       <c r="AN156">
         <v>3</v>
       </c>
+      <c r="AO156">
+        <v>3</v>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -21150,6 +21620,9 @@
       <c r="AN157">
         <v>16</v>
       </c>
+      <c r="AO157">
+        <v>16</v>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -21282,6 +21755,9 @@
       <c r="AN158">
         <v>2</v>
       </c>
+      <c r="AO158">
+        <v>3</v>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -21414,6 +21890,9 @@
       <c r="AN159">
         <v>4</v>
       </c>
+      <c r="AO159">
+        <v>4</v>
+      </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -21546,6 +22025,9 @@
       <c r="AN160">
         <v>0</v>
       </c>
+      <c r="AO160">
+        <v>0</v>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -21678,6 +22160,9 @@
       <c r="AN161">
         <v>0</v>
       </c>
+      <c r="AO161">
+        <v>0</v>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -21810,6 +22295,9 @@
       <c r="AN162">
         <v>2</v>
       </c>
+      <c r="AO162">
+        <v>2</v>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -21942,6 +22430,9 @@
       <c r="AN163">
         <v>0</v>
       </c>
+      <c r="AO163">
+        <v>0</v>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -22074,6 +22565,9 @@
       <c r="AN164">
         <v>0</v>
       </c>
+      <c r="AO164">
+        <v>0</v>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -22206,6 +22700,9 @@
       <c r="AN165">
         <v>1</v>
       </c>
+      <c r="AO165">
+        <v>1</v>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -22338,6 +22835,9 @@
       <c r="AN166">
         <v>0</v>
       </c>
+      <c r="AO166">
+        <v>0</v>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -22470,6 +22970,9 @@
       <c r="AN167">
         <v>1</v>
       </c>
+      <c r="AO167">
+        <v>1</v>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -22602,6 +23105,9 @@
       <c r="AN168">
         <v>5</v>
       </c>
+      <c r="AO168">
+        <v>5</v>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -22734,6 +23240,9 @@
       <c r="AN169">
         <v>2</v>
       </c>
+      <c r="AO169">
+        <v>2</v>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -22866,6 +23375,9 @@
       <c r="AN170">
         <v>1</v>
       </c>
+      <c r="AO170">
+        <v>1</v>
+      </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -22998,6 +23510,9 @@
       <c r="AN171">
         <v>3</v>
       </c>
+      <c r="AO171">
+        <v>3</v>
+      </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -23130,6 +23645,9 @@
       <c r="AN172">
         <v>2</v>
       </c>
+      <c r="AO172">
+        <v>2</v>
+      </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -23262,6 +23780,9 @@
       <c r="AN173">
         <v>13</v>
       </c>
+      <c r="AO173">
+        <v>13</v>
+      </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -23394,6 +23915,9 @@
       <c r="AN174">
         <v>36</v>
       </c>
+      <c r="AO174">
+        <v>36</v>
+      </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -23526,6 +24050,9 @@
       <c r="AN175">
         <v>1</v>
       </c>
+      <c r="AO175">
+        <v>1</v>
+      </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -23658,6 +24185,9 @@
       <c r="AN176">
         <v>8</v>
       </c>
+      <c r="AO176">
+        <v>8</v>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -23790,6 +24320,9 @@
       <c r="AN177">
         <v>2</v>
       </c>
+      <c r="AO177">
+        <v>2</v>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -23922,6 +24455,9 @@
       <c r="AN178">
         <v>6</v>
       </c>
+      <c r="AO178">
+        <v>6</v>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -24054,6 +24590,9 @@
       <c r="AN179">
         <v>4</v>
       </c>
+      <c r="AO179">
+        <v>4</v>
+      </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -24186,6 +24725,9 @@
       <c r="AN180">
         <v>12</v>
       </c>
+      <c r="AO180">
+        <v>12</v>
+      </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -24318,6 +24860,9 @@
       <c r="AN181">
         <v>11</v>
       </c>
+      <c r="AO181">
+        <v>11</v>
+      </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -24450,6 +24995,9 @@
       <c r="AN182">
         <v>2</v>
       </c>
+      <c r="AO182">
+        <v>2</v>
+      </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -24582,6 +25130,9 @@
       <c r="AN183">
         <v>1</v>
       </c>
+      <c r="AO183">
+        <v>1</v>
+      </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -24714,6 +25265,9 @@
       <c r="AN184">
         <v>0</v>
       </c>
+      <c r="AO184">
+        <v>0</v>
+      </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -24846,6 +25400,9 @@
       <c r="AN185">
         <v>1</v>
       </c>
+      <c r="AO185">
+        <v>1</v>
+      </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -24978,6 +25535,9 @@
       <c r="AN186">
         <v>9</v>
       </c>
+      <c r="AO186">
+        <v>9</v>
+      </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
@@ -25110,6 +25670,9 @@
       <c r="AN187">
         <v>0</v>
       </c>
+      <c r="AO187">
+        <v>0</v>
+      </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
@@ -25242,6 +25805,9 @@
       <c r="AN188">
         <v>0</v>
       </c>
+      <c r="AO188">
+        <v>0</v>
+      </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -25374,6 +25940,9 @@
       <c r="AN189">
         <v>0</v>
       </c>
+      <c r="AO189">
+        <v>0</v>
+      </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -25506,6 +26075,9 @@
       <c r="AN190">
         <v>25</v>
       </c>
+      <c r="AO190">
+        <v>25</v>
+      </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -25638,6 +26210,9 @@
       <c r="AN191">
         <v>20</v>
       </c>
+      <c r="AO191">
+        <v>20</v>
+      </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -25770,6 +26345,9 @@
       <c r="AN192">
         <v>57</v>
       </c>
+      <c r="AO192">
+        <v>57</v>
+      </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
@@ -25902,6 +26480,9 @@
       <c r="AN193">
         <v>38</v>
       </c>
+      <c r="AO193">
+        <v>38</v>
+      </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -26034,6 +26615,9 @@
       <c r="AN194">
         <v>36</v>
       </c>
+      <c r="AO194">
+        <v>36</v>
+      </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -26166,6 +26750,9 @@
       <c r="AN195">
         <v>10</v>
       </c>
+      <c r="AO195">
+        <v>10</v>
+      </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
@@ -26298,6 +26885,9 @@
       <c r="AN196">
         <v>40</v>
       </c>
+      <c r="AO196">
+        <v>40</v>
+      </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -26430,6 +27020,9 @@
       <c r="AN197">
         <v>4</v>
       </c>
+      <c r="AO197">
+        <v>4</v>
+      </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
@@ -26562,6 +27155,9 @@
       <c r="AN198">
         <v>22</v>
       </c>
+      <c r="AO198">
+        <v>23</v>
+      </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
@@ -26694,6 +27290,9 @@
       <c r="AN199">
         <v>2</v>
       </c>
+      <c r="AO199">
+        <v>2</v>
+      </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
@@ -26826,6 +27425,9 @@
       <c r="AN200">
         <v>5</v>
       </c>
+      <c r="AO200">
+        <v>5</v>
+      </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
@@ -26958,6 +27560,9 @@
       <c r="AN201">
         <v>2</v>
       </c>
+      <c r="AO201">
+        <v>2</v>
+      </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
@@ -27090,6 +27695,9 @@
       <c r="AN202">
         <v>1</v>
       </c>
+      <c r="AO202">
+        <v>1</v>
+      </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
@@ -27222,6 +27830,9 @@
       <c r="AN203">
         <v>5</v>
       </c>
+      <c r="AO203">
+        <v>5</v>
+      </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
@@ -27354,6 +27965,9 @@
       <c r="AN204">
         <v>0</v>
       </c>
+      <c r="AO204">
+        <v>0</v>
+      </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
@@ -27486,6 +28100,9 @@
       <c r="AN205">
         <v>1</v>
       </c>
+      <c r="AO205">
+        <v>1</v>
+      </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
@@ -27618,6 +28235,9 @@
       <c r="AN206">
         <v>1</v>
       </c>
+      <c r="AO206">
+        <v>1</v>
+      </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
@@ -27750,6 +28370,9 @@
       <c r="AN207">
         <v>0</v>
       </c>
+      <c r="AO207">
+        <v>0</v>
+      </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
@@ -27882,6 +28505,9 @@
       <c r="AN208">
         <v>0</v>
       </c>
+      <c r="AO208">
+        <v>0</v>
+      </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
@@ -28014,6 +28640,9 @@
       <c r="AN209">
         <v>0</v>
       </c>
+      <c r="AO209">
+        <v>0</v>
+      </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
@@ -28146,6 +28775,9 @@
       <c r="AN210">
         <v>0</v>
       </c>
+      <c r="AO210">
+        <v>0</v>
+      </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
@@ -28278,6 +28910,9 @@
       <c r="AN211">
         <v>0</v>
       </c>
+      <c r="AO211">
+        <v>0</v>
+      </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
@@ -28410,6 +29045,9 @@
       <c r="AN212">
         <v>2</v>
       </c>
+      <c r="AO212">
+        <v>2</v>
+      </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
@@ -28542,6 +29180,9 @@
       <c r="AN213">
         <v>0</v>
       </c>
+      <c r="AO213">
+        <v>0</v>
+      </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
@@ -28674,6 +29315,9 @@
       <c r="AN214">
         <v>3</v>
       </c>
+      <c r="AO214">
+        <v>3</v>
+      </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
@@ -28806,6 +29450,9 @@
       <c r="AN215">
         <v>30</v>
       </c>
+      <c r="AO215">
+        <v>30</v>
+      </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
@@ -28938,6 +29585,9 @@
       <c r="AN216">
         <v>216</v>
       </c>
+      <c r="AO216">
+        <v>217</v>
+      </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
@@ -29070,6 +29720,9 @@
       <c r="AN217">
         <v>9</v>
       </c>
+      <c r="AO217">
+        <v>9</v>
+      </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
@@ -29202,6 +29855,9 @@
       <c r="AN218">
         <v>11</v>
       </c>
+      <c r="AO218">
+        <v>11</v>
+      </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
@@ -29334,6 +29990,9 @@
       <c r="AN219">
         <v>0</v>
       </c>
+      <c r="AO219">
+        <v>0</v>
+      </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
@@ -29466,6 +30125,9 @@
       <c r="AN220">
         <v>2</v>
       </c>
+      <c r="AO220">
+        <v>2</v>
+      </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
@@ -29598,6 +30260,9 @@
       <c r="AN221">
         <v>0</v>
       </c>
+      <c r="AO221">
+        <v>0</v>
+      </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
@@ -29730,6 +30395,9 @@
       <c r="AN222">
         <v>1</v>
       </c>
+      <c r="AO222">
+        <v>1</v>
+      </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
@@ -29862,6 +30530,9 @@
       <c r="AN223">
         <v>2</v>
       </c>
+      <c r="AO223">
+        <v>2</v>
+      </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
@@ -29994,6 +30665,9 @@
       <c r="AN224">
         <v>8</v>
       </c>
+      <c r="AO224">
+        <v>8</v>
+      </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
@@ -30126,6 +30800,9 @@
       <c r="AN225">
         <v>3</v>
       </c>
+      <c r="AO225">
+        <v>3</v>
+      </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
@@ -30258,6 +30935,9 @@
       <c r="AN226">
         <v>1</v>
       </c>
+      <c r="AO226">
+        <v>1</v>
+      </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
@@ -30390,6 +31070,9 @@
       <c r="AN227">
         <v>2</v>
       </c>
+      <c r="AO227">
+        <v>2</v>
+      </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
@@ -30522,6 +31205,9 @@
       <c r="AN228">
         <v>2</v>
       </c>
+      <c r="AO228">
+        <v>2</v>
+      </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
@@ -30654,6 +31340,9 @@
       <c r="AN229">
         <v>2</v>
       </c>
+      <c r="AO229">
+        <v>2</v>
+      </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
@@ -30786,6 +31475,9 @@
       <c r="AN230">
         <v>0</v>
       </c>
+      <c r="AO230">
+        <v>0</v>
+      </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
@@ -30918,6 +31610,9 @@
       <c r="AN231">
         <v>3</v>
       </c>
+      <c r="AO231">
+        <v>3</v>
+      </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
@@ -31050,6 +31745,9 @@
       <c r="AN232">
         <v>21</v>
       </c>
+      <c r="AO232">
+        <v>21</v>
+      </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
@@ -31182,6 +31880,9 @@
       <c r="AN233">
         <v>0</v>
       </c>
+      <c r="AO233">
+        <v>0</v>
+      </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
@@ -31314,6 +32015,9 @@
       <c r="AN234">
         <v>4</v>
       </c>
+      <c r="AO234">
+        <v>4</v>
+      </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
@@ -31446,6 +32150,9 @@
       <c r="AN235">
         <v>1</v>
       </c>
+      <c r="AO235">
+        <v>1</v>
+      </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
@@ -31578,6 +32285,9 @@
       <c r="AN236">
         <v>1</v>
       </c>
+      <c r="AO236">
+        <v>1</v>
+      </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
@@ -31710,6 +32420,9 @@
       <c r="AN237">
         <v>1</v>
       </c>
+      <c r="AO237">
+        <v>1</v>
+      </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
@@ -31842,6 +32555,9 @@
       <c r="AN238">
         <v>533</v>
       </c>
+      <c r="AO238">
+        <v>544</v>
+      </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
@@ -31974,6 +32690,9 @@
       <c r="AN239">
         <v>9</v>
       </c>
+      <c r="AO239">
+        <v>9</v>
+      </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
@@ -32106,6 +32825,9 @@
       <c r="AN240">
         <v>4</v>
       </c>
+      <c r="AO240">
+        <v>4</v>
+      </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
@@ -32238,6 +32960,9 @@
       <c r="AN241">
         <v>4</v>
       </c>
+      <c r="AO241">
+        <v>4</v>
+      </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
@@ -32370,6 +33095,9 @@
       <c r="AN242">
         <v>4</v>
       </c>
+      <c r="AO242">
+        <v>4</v>
+      </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
@@ -32502,6 +33230,9 @@
       <c r="AN243">
         <v>6</v>
       </c>
+      <c r="AO243">
+        <v>6</v>
+      </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
@@ -32634,6 +33365,9 @@
       <c r="AN244">
         <v>8</v>
       </c>
+      <c r="AO244">
+        <v>8</v>
+      </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
@@ -32766,6 +33500,9 @@
       <c r="AN245">
         <v>0</v>
       </c>
+      <c r="AO245">
+        <v>0</v>
+      </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
@@ -32898,6 +33635,9 @@
       <c r="AN246">
         <v>4</v>
       </c>
+      <c r="AO246">
+        <v>4</v>
+      </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
@@ -33030,6 +33770,9 @@
       <c r="AN247">
         <v>0</v>
       </c>
+      <c r="AO247">
+        <v>0</v>
+      </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
@@ -33162,6 +33905,9 @@
       <c r="AN248">
         <v>0</v>
       </c>
+      <c r="AO248">
+        <v>0</v>
+      </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
@@ -33294,6 +34040,9 @@
       <c r="AN249">
         <v>2</v>
       </c>
+      <c r="AO249">
+        <v>2</v>
+      </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
@@ -33426,6 +34175,9 @@
       <c r="AN250">
         <v>24</v>
       </c>
+      <c r="AO250">
+        <v>24</v>
+      </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
@@ -33558,6 +34310,9 @@
       <c r="AN251">
         <v>9</v>
       </c>
+      <c r="AO251">
+        <v>9</v>
+      </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
@@ -33690,6 +34445,9 @@
       <c r="AN252">
         <v>0</v>
       </c>
+      <c r="AO252">
+        <v>0</v>
+      </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
@@ -33822,6 +34580,9 @@
       <c r="AN253">
         <v>17</v>
       </c>
+      <c r="AO253">
+        <v>17</v>
+      </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
@@ -33954,6 +34715,9 @@
       <c r="AN254">
         <v>5</v>
       </c>
+      <c r="AO254">
+        <v>5</v>
+      </c>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
@@ -34086,6 +34850,9 @@
       <c r="AN255">
         <v>53</v>
       </c>
+      <c r="AO255">
+        <v>53</v>
+      </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
@@ -34218,6 +34985,9 @@
       <c r="AN256">
         <v>40</v>
       </c>
+      <c r="AO256">
+        <v>41</v>
+      </c>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
@@ -34350,6 +35120,9 @@
       <c r="AN257">
         <v>1</v>
       </c>
+      <c r="AO257">
+        <v>1</v>
+      </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
@@ -34482,6 +35255,9 @@
       <c r="AN258">
         <v>0</v>
       </c>
+      <c r="AO258">
+        <v>0</v>
+      </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
@@ -34614,6 +35390,9 @@
       <c r="AN259">
         <v>40</v>
       </c>
+      <c r="AO259">
+        <v>40</v>
+      </c>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
@@ -34746,6 +35525,9 @@
       <c r="AN260">
         <v>26</v>
       </c>
+      <c r="AO260">
+        <v>26</v>
+      </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
@@ -34878,6 +35660,9 @@
       <c r="AN261">
         <v>0</v>
       </c>
+      <c r="AO261">
+        <v>0</v>
+      </c>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
@@ -35010,6 +35795,9 @@
       <c r="AN262">
         <v>0</v>
       </c>
+      <c r="AO262">
+        <v>0</v>
+      </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
@@ -35142,6 +35930,9 @@
       <c r="AN263">
         <v>0</v>
       </c>
+      <c r="AO263">
+        <v>0</v>
+      </c>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
@@ -35274,6 +36065,9 @@
       <c r="AN264">
         <v>1</v>
       </c>
+      <c r="AO264">
+        <v>1</v>
+      </c>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
@@ -35406,6 +36200,9 @@
       <c r="AN265">
         <v>3</v>
       </c>
+      <c r="AO265">
+        <v>3</v>
+      </c>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
@@ -35538,6 +36335,9 @@
       <c r="AN266">
         <v>0</v>
       </c>
+      <c r="AO266">
+        <v>0</v>
+      </c>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
@@ -35670,6 +36470,9 @@
       <c r="AN267">
         <v>3</v>
       </c>
+      <c r="AO267">
+        <v>3</v>
+      </c>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
@@ -35802,6 +36605,9 @@
       <c r="AN268">
         <v>0</v>
       </c>
+      <c r="AO268">
+        <v>0</v>
+      </c>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
@@ -35934,6 +36740,9 @@
       <c r="AN269">
         <v>7</v>
       </c>
+      <c r="AO269">
+        <v>7</v>
+      </c>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
@@ -36066,6 +36875,9 @@
       <c r="AN270">
         <v>0</v>
       </c>
+      <c r="AO270">
+        <v>0</v>
+      </c>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
@@ -36198,6 +37010,9 @@
       <c r="AN271">
         <v>0</v>
       </c>
+      <c r="AO271">
+        <v>0</v>
+      </c>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
@@ -36330,6 +37145,9 @@
       <c r="AN272">
         <v>1</v>
       </c>
+      <c r="AO272">
+        <v>1</v>
+      </c>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
@@ -36462,6 +37280,9 @@
       <c r="AN273">
         <v>4</v>
       </c>
+      <c r="AO273">
+        <v>4</v>
+      </c>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
@@ -36594,6 +37415,9 @@
       <c r="AN274">
         <v>0</v>
       </c>
+      <c r="AO274">
+        <v>0</v>
+      </c>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
@@ -36726,6 +37550,9 @@
       <c r="AN275">
         <v>0</v>
       </c>
+      <c r="AO275">
+        <v>0</v>
+      </c>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
@@ -36858,6 +37685,9 @@
       <c r="AN276">
         <v>17</v>
       </c>
+      <c r="AO276">
+        <v>17</v>
+      </c>
     </row>
     <row r="277">
       <c r="A277" t="inlineStr">
@@ -36990,6 +37820,9 @@
       <c r="AN277">
         <v>0</v>
       </c>
+      <c r="AO277">
+        <v>0</v>
+      </c>
     </row>
     <row r="278">
       <c r="A278" t="inlineStr">
@@ -37122,6 +37955,9 @@
       <c r="AN278">
         <v>0</v>
       </c>
+      <c r="AO278">
+        <v>0</v>
+      </c>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
@@ -37254,6 +38090,9 @@
       <c r="AN279">
         <v>4</v>
       </c>
+      <c r="AO279">
+        <v>4</v>
+      </c>
     </row>
     <row r="280">
       <c r="A280" t="inlineStr">
@@ -37386,6 +38225,9 @@
       <c r="AN280">
         <v>12</v>
       </c>
+      <c r="AO280">
+        <v>12</v>
+      </c>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr">
@@ -37518,6 +38360,9 @@
       <c r="AN281">
         <v>279</v>
       </c>
+      <c r="AO281">
+        <v>280</v>
+      </c>
     </row>
     <row r="282">
       <c r="A282" t="inlineStr">
@@ -37650,6 +38495,9 @@
       <c r="AN282">
         <v>16</v>
       </c>
+      <c r="AO282">
+        <v>16</v>
+      </c>
     </row>
     <row r="283">
       <c r="A283" t="inlineStr">
@@ -37782,6 +38630,9 @@
       <c r="AN283">
         <v>5</v>
       </c>
+      <c r="AO283">
+        <v>5</v>
+      </c>
     </row>
     <row r="284">
       <c r="A284" t="inlineStr">
@@ -37914,6 +38765,9 @@
       <c r="AN284">
         <v>0</v>
       </c>
+      <c r="AO284">
+        <v>0</v>
+      </c>
     </row>
     <row r="285">
       <c r="A285" t="inlineStr">
@@ -38046,6 +38900,9 @@
       <c r="AN285">
         <v>0</v>
       </c>
+      <c r="AO285">
+        <v>0</v>
+      </c>
     </row>
     <row r="286">
       <c r="A286" t="inlineStr">
@@ -38178,6 +39035,9 @@
       <c r="AN286">
         <v>8</v>
       </c>
+      <c r="AO286">
+        <v>8</v>
+      </c>
     </row>
     <row r="287">
       <c r="A287" t="inlineStr">
@@ -38310,6 +39170,9 @@
       <c r="AN287">
         <v>5</v>
       </c>
+      <c r="AO287">
+        <v>5</v>
+      </c>
     </row>
     <row r="288">
       <c r="A288" t="inlineStr">
@@ -38442,6 +39305,9 @@
       <c r="AN288">
         <v>0</v>
       </c>
+      <c r="AO288">
+        <v>0</v>
+      </c>
     </row>
     <row r="289">
       <c r="A289" t="inlineStr">
@@ -38574,6 +39440,9 @@
       <c r="AN289">
         <v>1</v>
       </c>
+      <c r="AO289">
+        <v>1</v>
+      </c>
     </row>
     <row r="290">
       <c r="A290" t="inlineStr">
@@ -38706,6 +39575,9 @@
       <c r="AN290">
         <v>7</v>
       </c>
+      <c r="AO290">
+        <v>7</v>
+      </c>
     </row>
     <row r="291">
       <c r="A291" t="inlineStr">
@@ -38838,6 +39710,9 @@
       <c r="AN291">
         <v>3</v>
       </c>
+      <c r="AO291">
+        <v>3</v>
+      </c>
     </row>
     <row r="292">
       <c r="A292" t="inlineStr">
@@ -38970,6 +39845,9 @@
       <c r="AN292">
         <v>5</v>
       </c>
+      <c r="AO292">
+        <v>5</v>
+      </c>
     </row>
     <row r="293">
       <c r="A293" t="inlineStr">
@@ -39102,6 +39980,9 @@
       <c r="AN293">
         <v>12</v>
       </c>
+      <c r="AO293">
+        <v>12</v>
+      </c>
     </row>
     <row r="294">
       <c r="A294" t="inlineStr">
@@ -39234,6 +40115,9 @@
       <c r="AN294">
         <v>6</v>
       </c>
+      <c r="AO294">
+        <v>6</v>
+      </c>
     </row>
     <row r="295">
       <c r="A295" t="inlineStr">
@@ -39366,6 +40250,9 @@
       <c r="AN295">
         <v>0</v>
       </c>
+      <c r="AO295">
+        <v>0</v>
+      </c>
     </row>
     <row r="296">
       <c r="A296" t="inlineStr">
@@ -39498,6 +40385,9 @@
       <c r="AN296">
         <v>1</v>
       </c>
+      <c r="AO296">
+        <v>1</v>
+      </c>
     </row>
     <row r="297">
       <c r="A297" t="inlineStr">
@@ -39630,6 +40520,9 @@
       <c r="AN297">
         <v>8</v>
       </c>
+      <c r="AO297">
+        <v>8</v>
+      </c>
     </row>
     <row r="298">
       <c r="A298" t="inlineStr">
@@ -39762,6 +40655,9 @@
       <c r="AN298">
         <v>28</v>
       </c>
+      <c r="AO298">
+        <v>28</v>
+      </c>
     </row>
     <row r="299">
       <c r="A299" t="inlineStr">
@@ -39894,6 +40790,9 @@
       <c r="AN299">
         <v>21</v>
       </c>
+      <c r="AO299">
+        <v>21</v>
+      </c>
     </row>
     <row r="300">
       <c r="A300" t="inlineStr">
@@ -40026,6 +40925,9 @@
       <c r="AN300">
         <v>15</v>
       </c>
+      <c r="AO300">
+        <v>15</v>
+      </c>
     </row>
     <row r="301">
       <c r="A301" t="inlineStr">
@@ -40158,6 +41060,9 @@
       <c r="AN301">
         <v>1</v>
       </c>
+      <c r="AO301">
+        <v>1</v>
+      </c>
     </row>
     <row r="302">
       <c r="A302" t="inlineStr">
@@ -40290,6 +41195,9 @@
       <c r="AN302">
         <v>0</v>
       </c>
+      <c r="AO302">
+        <v>0</v>
+      </c>
     </row>
     <row r="303">
       <c r="A303" t="inlineStr">
@@ -40422,6 +41330,9 @@
       <c r="AN303">
         <v>0</v>
       </c>
+      <c r="AO303">
+        <v>0</v>
+      </c>
     </row>
     <row r="304">
       <c r="A304" t="inlineStr">
@@ -40554,6 +41465,9 @@
       <c r="AN304">
         <v>0</v>
       </c>
+      <c r="AO304">
+        <v>0</v>
+      </c>
     </row>
     <row r="305">
       <c r="A305" t="inlineStr">
@@ -40686,6 +41600,9 @@
       <c r="AN305">
         <v>3</v>
       </c>
+      <c r="AO305">
+        <v>3</v>
+      </c>
     </row>
     <row r="306">
       <c r="A306" t="inlineStr">
@@ -40818,6 +41735,9 @@
       <c r="AN306">
         <v>1</v>
       </c>
+      <c r="AO306">
+        <v>1</v>
+      </c>
     </row>
     <row r="307">
       <c r="A307" t="inlineStr">
@@ -40950,6 +41870,9 @@
       <c r="AN307">
         <v>4</v>
       </c>
+      <c r="AO307">
+        <v>4</v>
+      </c>
     </row>
     <row r="308">
       <c r="A308" t="inlineStr">
@@ -41082,6 +42005,9 @@
       <c r="AN308">
         <v>0</v>
       </c>
+      <c r="AO308">
+        <v>0</v>
+      </c>
     </row>
     <row r="309">
       <c r="A309" t="inlineStr">
@@ -41214,6 +42140,9 @@
       <c r="AN309">
         <v>0</v>
       </c>
+      <c r="AO309">
+        <v>0</v>
+      </c>
     </row>
     <row r="310">
       <c r="A310" t="inlineStr">
@@ -41346,6 +42275,9 @@
       <c r="AN310">
         <v>7</v>
       </c>
+      <c r="AO310">
+        <v>7</v>
+      </c>
     </row>
     <row r="311">
       <c r="A311" t="inlineStr">
@@ -41478,6 +42410,9 @@
       <c r="AN311">
         <v>2</v>
       </c>
+      <c r="AO311">
+        <v>2</v>
+      </c>
     </row>
     <row r="312">
       <c r="A312" t="inlineStr">
@@ -41610,6 +42545,9 @@
       <c r="AN312">
         <v>2</v>
       </c>
+      <c r="AO312">
+        <v>2</v>
+      </c>
     </row>
     <row r="313">
       <c r="A313" t="inlineStr">
@@ -41742,6 +42680,9 @@
       <c r="AN313">
         <v>2</v>
       </c>
+      <c r="AO313">
+        <v>2</v>
+      </c>
     </row>
     <row r="314">
       <c r="A314" t="inlineStr">
@@ -41874,6 +42815,9 @@
       <c r="AN314">
         <v>10</v>
       </c>
+      <c r="AO314">
+        <v>10</v>
+      </c>
     </row>
     <row r="315">
       <c r="A315" t="inlineStr">
@@ -42006,6 +42950,9 @@
       <c r="AN315">
         <v>1</v>
       </c>
+      <c r="AO315">
+        <v>1</v>
+      </c>
     </row>
     <row r="316">
       <c r="A316" t="inlineStr">
@@ -42138,6 +43085,9 @@
       <c r="AN316">
         <v>17</v>
       </c>
+      <c r="AO316">
+        <v>17</v>
+      </c>
     </row>
     <row r="317">
       <c r="A317" t="inlineStr">
@@ -42270,6 +43220,9 @@
       <c r="AN317">
         <v>0</v>
       </c>
+      <c r="AO317">
+        <v>0</v>
+      </c>
     </row>
     <row r="318">
       <c r="A318" t="inlineStr">
@@ -42402,6 +43355,9 @@
       <c r="AN318">
         <v>0</v>
       </c>
+      <c r="AO318">
+        <v>0</v>
+      </c>
     </row>
     <row r="319">
       <c r="A319" t="inlineStr">
@@ -42534,6 +43490,9 @@
       <c r="AN319">
         <v>152</v>
       </c>
+      <c r="AO319">
+        <v>155</v>
+      </c>
     </row>
     <row r="320">
       <c r="A320" t="inlineStr">
@@ -42666,6 +43625,9 @@
       <c r="AN320">
         <v>6</v>
       </c>
+      <c r="AO320">
+        <v>6</v>
+      </c>
     </row>
     <row r="321">
       <c r="A321" t="inlineStr">
@@ -42798,6 +43760,9 @@
       <c r="AN321">
         <v>5</v>
       </c>
+      <c r="AO321">
+        <v>5</v>
+      </c>
     </row>
     <row r="322">
       <c r="A322" t="inlineStr">
@@ -42930,6 +43895,9 @@
       <c r="AN322">
         <v>1</v>
       </c>
+      <c r="AO322">
+        <v>1</v>
+      </c>
     </row>
     <row r="323">
       <c r="A323" t="inlineStr">
@@ -43062,6 +44030,9 @@
       <c r="AN323">
         <v>3</v>
       </c>
+      <c r="AO323">
+        <v>3</v>
+      </c>
     </row>
     <row r="324">
       <c r="A324" t="inlineStr">
@@ -43194,6 +44165,9 @@
       <c r="AN324">
         <v>15</v>
       </c>
+      <c r="AO324">
+        <v>15</v>
+      </c>
     </row>
     <row r="325">
       <c r="A325" t="inlineStr">
@@ -43326,6 +44300,9 @@
       <c r="AN325">
         <v>1</v>
       </c>
+      <c r="AO325">
+        <v>1</v>
+      </c>
     </row>
     <row r="326">
       <c r="A326" t="inlineStr">
@@ -43458,6 +44435,9 @@
       <c r="AN326">
         <v>1</v>
       </c>
+      <c r="AO326">
+        <v>1</v>
+      </c>
     </row>
     <row r="327">
       <c r="A327" t="inlineStr">
@@ -43590,6 +44570,9 @@
       <c r="AN327">
         <v>0</v>
       </c>
+      <c r="AO327">
+        <v>0</v>
+      </c>
     </row>
     <row r="328">
       <c r="A328" t="inlineStr">
@@ -43722,6 +44705,9 @@
       <c r="AN328">
         <v>0</v>
       </c>
+      <c r="AO328">
+        <v>0</v>
+      </c>
     </row>
     <row r="329">
       <c r="A329" t="inlineStr">
@@ -43854,6 +44840,9 @@
       <c r="AN329">
         <v>3</v>
       </c>
+      <c r="AO329">
+        <v>3</v>
+      </c>
     </row>
     <row r="330">
       <c r="A330" t="inlineStr">
@@ -43986,6 +44975,9 @@
       <c r="AN330">
         <v>1</v>
       </c>
+      <c r="AO330">
+        <v>1</v>
+      </c>
     </row>
     <row r="331">
       <c r="A331" t="inlineStr">
@@ -44118,6 +45110,9 @@
       <c r="AN331">
         <v>2</v>
       </c>
+      <c r="AO331">
+        <v>2</v>
+      </c>
     </row>
     <row r="332">
       <c r="A332" t="inlineStr">
@@ -44250,6 +45245,9 @@
       <c r="AN332">
         <v>1</v>
       </c>
+      <c r="AO332">
+        <v>1</v>
+      </c>
     </row>
     <row r="333">
       <c r="A333" t="inlineStr">
@@ -44382,6 +45380,9 @@
       <c r="AN333">
         <v>0</v>
       </c>
+      <c r="AO333">
+        <v>0</v>
+      </c>
     </row>
     <row r="334">
       <c r="A334" t="inlineStr">
@@ -44514,6 +45515,9 @@
       <c r="AN334">
         <v>0</v>
       </c>
+      <c r="AO334">
+        <v>0</v>
+      </c>
     </row>
     <row r="335">
       <c r="A335" t="inlineStr">
@@ -44646,6 +45650,9 @@
       <c r="AN335">
         <v>16</v>
       </c>
+      <c r="AO335">
+        <v>16</v>
+      </c>
     </row>
     <row r="336">
       <c r="A336" t="inlineStr">
@@ -44778,6 +45785,9 @@
       <c r="AN336">
         <v>2</v>
       </c>
+      <c r="AO336">
+        <v>2</v>
+      </c>
     </row>
     <row r="337">
       <c r="A337" t="inlineStr">
@@ -44910,6 +45920,9 @@
       <c r="AN337">
         <v>1</v>
       </c>
+      <c r="AO337">
+        <v>1</v>
+      </c>
     </row>
     <row r="338">
       <c r="A338" t="inlineStr">
@@ -45042,6 +46055,9 @@
       <c r="AN338">
         <v>2</v>
       </c>
+      <c r="AO338">
+        <v>2</v>
+      </c>
     </row>
     <row r="339">
       <c r="A339" t="inlineStr">
@@ -45174,6 +46190,9 @@
       <c r="AN339">
         <v>0</v>
       </c>
+      <c r="AO339">
+        <v>0</v>
+      </c>
     </row>
     <row r="340">
       <c r="A340" t="inlineStr">
@@ -45306,6 +46325,9 @@
       <c r="AN340">
         <v>0</v>
       </c>
+      <c r="AO340">
+        <v>0</v>
+      </c>
     </row>
     <row r="341">
       <c r="A341" t="inlineStr">
@@ -45438,6 +46460,9 @@
       <c r="AN341">
         <v>1</v>
       </c>
+      <c r="AO341">
+        <v>1</v>
+      </c>
     </row>
     <row r="342">
       <c r="A342" t="inlineStr">
@@ -45570,6 +46595,9 @@
       <c r="AN342">
         <v>2</v>
       </c>
+      <c r="AO342">
+        <v>2</v>
+      </c>
     </row>
     <row r="343">
       <c r="A343" t="inlineStr">
@@ -45702,6 +46730,9 @@
       <c r="AN343">
         <v>0</v>
       </c>
+      <c r="AO343">
+        <v>0</v>
+      </c>
     </row>
     <row r="344">
       <c r="A344" t="inlineStr">
@@ -45834,6 +46865,9 @@
       <c r="AN344">
         <v>1</v>
       </c>
+      <c r="AO344">
+        <v>1</v>
+      </c>
     </row>
     <row r="345">
       <c r="A345" t="inlineStr">
@@ -45966,6 +47000,9 @@
       <c r="AN345">
         <v>0</v>
       </c>
+      <c r="AO345">
+        <v>0</v>
+      </c>
     </row>
     <row r="346">
       <c r="A346" t="inlineStr">
@@ -46098,6 +47135,9 @@
       <c r="AN346">
         <v>0</v>
       </c>
+      <c r="AO346">
+        <v>0</v>
+      </c>
     </row>
     <row r="347">
       <c r="A347" t="inlineStr">
@@ -46230,6 +47270,9 @@
       <c r="AN347">
         <v>3</v>
       </c>
+      <c r="AO347">
+        <v>3</v>
+      </c>
     </row>
     <row r="348">
       <c r="A348" t="inlineStr">
@@ -46362,6 +47405,9 @@
       <c r="AN348">
         <v>2</v>
       </c>
+      <c r="AO348">
+        <v>2</v>
+      </c>
     </row>
     <row r="349">
       <c r="A349" t="inlineStr">
@@ -46494,6 +47540,9 @@
       <c r="AN349">
         <v>4</v>
       </c>
+      <c r="AO349">
+        <v>4</v>
+      </c>
     </row>
     <row r="350">
       <c r="A350" t="inlineStr">
@@ -46626,6 +47675,9 @@
       <c r="AN350">
         <v>1</v>
       </c>
+      <c r="AO350">
+        <v>1</v>
+      </c>
     </row>
     <row r="351">
       <c r="A351" t="inlineStr">
@@ -46758,6 +47810,9 @@
       <c r="AN351">
         <v>0</v>
       </c>
+      <c r="AO351">
+        <v>0</v>
+      </c>
     </row>
     <row r="352">
       <c r="A352" t="inlineStr">
@@ -46890,6 +47945,9 @@
       <c r="AN352">
         <v>0</v>
       </c>
+      <c r="AO352">
+        <v>0</v>
+      </c>
     </row>
     <row r="353">
       <c r="A353" t="inlineStr">
@@ -47022,6 +48080,9 @@
       <c r="AN353">
         <v>0</v>
       </c>
+      <c r="AO353">
+        <v>0</v>
+      </c>
     </row>
     <row r="354">
       <c r="A354" t="inlineStr">
@@ -47154,6 +48215,9 @@
       <c r="AN354">
         <v>1</v>
       </c>
+      <c r="AO354">
+        <v>1</v>
+      </c>
     </row>
     <row r="355">
       <c r="A355" t="inlineStr">
@@ -47286,6 +48350,9 @@
       <c r="AN355">
         <v>1</v>
       </c>
+      <c r="AO355">
+        <v>1</v>
+      </c>
     </row>
     <row r="356">
       <c r="A356" t="inlineStr">
@@ -47418,6 +48485,9 @@
       <c r="AN356">
         <v>0</v>
       </c>
+      <c r="AO356">
+        <v>0</v>
+      </c>
     </row>
     <row r="357">
       <c r="A357" t="inlineStr">
@@ -47550,6 +48620,9 @@
       <c r="AN357">
         <v>4</v>
       </c>
+      <c r="AO357">
+        <v>4</v>
+      </c>
     </row>
     <row r="358">
       <c r="A358" t="inlineStr">
@@ -47682,6 +48755,9 @@
       <c r="AN358">
         <v>0</v>
       </c>
+      <c r="AO358">
+        <v>0</v>
+      </c>
     </row>
     <row r="359">
       <c r="A359" t="inlineStr">
@@ -47812,6 +48888,9 @@
         <v>0</v>
       </c>
       <c r="AN359">
+        <v>0</v>
+      </c>
+      <c r="AO359">
         <v>0</v>
       </c>
     </row>

</xml_diff>